<commit_message>
Excel shared string table parsing and CSV export
</commit_message>
<xml_diff>
--- a/test/content/simple_test.xlsx
+++ b/test/content/simple_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Heading A</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Bravo</t>
+  </si>
+  <si>
+    <t>a;b;c;d</t>
   </si>
 </sst>
 </file>
@@ -414,9 +417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -445,8 +446,8 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="C4" s="1">
-        <v>29399</v>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>